<commit_message>
new table classes and formatting
</commit_message>
<xml_diff>
--- a/data/tables/IA_BLE_Tracking_template.xlsx
+++ b/data/tables/IA_BLE_Tracking_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\automation\toolboxes\IA_BLE_tracking\data\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/PycharmProjects/IA_BLE_tracking/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE5591D-4164-42D7-B770-3A721E8B36A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8622AF27-E2DF-C44D-8CE7-CD4570F972FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12200" yWindow="500" windowWidth="24340" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking_Main" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="194">
   <si>
     <t>HUC8</t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t>Source Columns</t>
+  </si>
+  <si>
+    <t>TO Area</t>
+  </si>
+  <si>
+    <t>MIP Case</t>
   </si>
 </sst>
 </file>
@@ -650,6 +656,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -674,7 +681,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -813,6 +820,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -826,7 +848,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -867,14 +888,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,32 +1204,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="43" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>181</v>
       </c>
@@ -1223,7 +1247,7 @@
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
       <c r="K1" s="22"/>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="19" t="s">
         <v>187</v>
       </c>
       <c r="M1" s="20" t="s">
@@ -1237,94 +1261,94 @@
       </c>
       <c r="R1" s="22"/>
     </row>
-    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:18" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -1333,54 +1357,54 @@
       <c r="M3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3">
         <v>100</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1389,54 +1413,54 @@
       <c r="M4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4">
         <v>100</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1445,54 +1469,54 @@
       <c r="M5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5">
         <v>100</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1501,54 +1525,54 @@
       <c r="M6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6">
         <v>100</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="R6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1557,54 +1581,54 @@
       <c r="M7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7">
         <v>100</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1613,52 +1637,51 @@
       <c r="M8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8">
         <v>100</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>66</v>
       </c>
       <c r="L9" s="3" t="s">
@@ -1667,52 +1690,52 @@
       <c r="M9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" t="s">
         <v>48</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="14" t="s">
+      <c r="P9" s="8"/>
+      <c r="Q9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L10" s="3" t="s">
@@ -1721,50 +1744,48 @@
       <c r="M10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" t="s">
         <v>80</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10">
         <v>100</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="R10" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>83</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -1773,48 +1794,46 @@
       <c r="M11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" t="s">
         <v>86</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="14" t="s">
+      <c r="P11" s="8"/>
+      <c r="Q11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="R11" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>83</v>
       </c>
       <c r="L12" s="3" t="s">
@@ -1823,50 +1842,48 @@
       <c r="M12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" t="s">
         <v>91</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="P12" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="R12" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>83</v>
       </c>
       <c r="L13" s="3" t="s">
@@ -1875,50 +1892,49 @@
       <c r="M13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="4">
+      <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="14" t="s">
+      <c r="P13" s="8"/>
+      <c r="Q13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="R13" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" t="s">
         <v>99</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>83</v>
       </c>
       <c r="L14" s="3" t="s">
@@ -1927,52 +1943,52 @@
       <c r="M14" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N14" t="s">
         <v>101</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="14" t="s">
+      <c r="P14" s="8"/>
+      <c r="Q14" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="R14" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" t="s">
         <v>106</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" t="s">
         <v>107</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="3" t="s">
@@ -1981,54 +1997,54 @@
       <c r="M15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" t="s">
         <v>110</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15">
         <v>100</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="P15" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="5" t="s">
+      <c r="R15" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" t="s">
         <v>116</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" t="s">
         <v>117</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L16" s="3" t="s">
@@ -2037,54 +2053,54 @@
       <c r="M16" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" t="s">
         <v>78</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16">
         <v>100</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R16" s="5" t="s">
+      <c r="R16" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" t="s">
         <v>120</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" t="s">
         <v>123</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -2093,54 +2109,54 @@
       <c r="M17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" t="s">
         <v>124</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17">
         <v>100</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R17" s="5" t="s">
+      <c r="R17" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" t="s">
         <v>128</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" t="s">
         <v>129</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" t="s">
         <v>129</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -2149,54 +2165,54 @@
       <c r="M18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" t="s">
         <v>110</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18">
         <v>100</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" t="s">
         <v>117</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" t="s">
         <v>117</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L19" s="3" t="s">
@@ -2205,54 +2221,54 @@
       <c r="M19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="N19" t="s">
         <v>134</v>
       </c>
-      <c r="O19" s="4">
+      <c r="O19">
         <v>100</v>
       </c>
-      <c r="P19" s="9" t="s">
+      <c r="P19" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q19" s="14" t="s">
+      <c r="Q19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="R19" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" t="s">
         <v>138</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" t="s">
         <v>139</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" t="s">
         <v>139</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -2261,54 +2277,54 @@
       <c r="M20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N20" s="4" t="s">
+      <c r="N20" t="s">
         <v>62</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20">
         <v>100</v>
       </c>
-      <c r="P20" s="9" t="s">
+      <c r="P20" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="Q20" s="14" t="s">
+      <c r="Q20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="5" t="s">
+      <c r="R20" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" t="s">
         <v>144</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" t="s">
         <v>145</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L21" s="3" t="s">
@@ -2317,54 +2333,54 @@
       <c r="M21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N21" t="s">
         <v>48</v>
       </c>
-      <c r="O21" s="4">
+      <c r="O21">
         <v>100</v>
       </c>
-      <c r="P21" s="9" t="s">
+      <c r="P21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" s="14" t="s">
+      <c r="Q21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="R21" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>148</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" t="s">
         <v>150</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" t="s">
         <v>147</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" t="s">
         <v>147</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -2373,54 +2389,54 @@
       <c r="M22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="N22" t="s">
         <v>151</v>
       </c>
-      <c r="O22" s="4">
+      <c r="O22">
         <v>100</v>
       </c>
-      <c r="P22" s="9" t="s">
+      <c r="P22" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q22" s="14" t="s">
+      <c r="Q22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R22" s="5" t="s">
+      <c r="R22" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" t="s">
         <v>155</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" t="s">
         <v>123</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L23" s="3" t="s">
@@ -2429,54 +2445,54 @@
       <c r="M23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N23" t="s">
         <v>120</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O23">
         <v>100</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q23" s="14" t="s">
+      <c r="Q23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R23" s="5" t="s">
+      <c r="R23" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" t="s">
         <v>155</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" t="s">
         <v>158</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L24" s="3" t="s">
@@ -2485,54 +2501,54 @@
       <c r="M24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="N24" t="s">
         <v>159</v>
       </c>
-      <c r="O24" s="4">
+      <c r="O24">
         <v>100</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="P24" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q24" s="14" t="s">
+      <c r="Q24" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R24" s="5" t="s">
+      <c r="R24" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>162</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="5" t="s">
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>148</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" t="s">
         <v>163</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" t="s">
         <v>164</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" t="s">
         <v>163</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -2541,54 +2557,54 @@
       <c r="M25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="N25" t="s">
         <v>151</v>
       </c>
-      <c r="O25" s="4">
+      <c r="O25">
         <v>100</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Q25" s="14" t="s">
+      <c r="Q25" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R25" s="5" t="s">
+      <c r="R25" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" t="s">
         <v>143</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" t="s">
         <v>164</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L26" s="3" t="s">
@@ -2597,54 +2613,54 @@
       <c r="M26" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N26" t="s">
         <v>53</v>
       </c>
-      <c r="O26" s="4">
+      <c r="O26">
         <v>100</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="P26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q26" s="14" t="s">
+      <c r="Q26" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R26" s="5" t="s">
+      <c r="R26" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" t="s">
         <v>170</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" t="s">
         <v>171</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L27" s="3" t="s">
@@ -2653,73 +2669,73 @@
       <c r="M27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="N27" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="4">
+      <c r="O27">
         <v>100</v>
       </c>
-      <c r="P27" s="9" t="s">
+      <c r="P27" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q27" s="14" t="s">
+      <c r="Q27" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R27" s="5" t="s">
+      <c r="R27" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J28" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="L28" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="M28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N28" s="7" t="s">
+      <c r="N28" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="6">
         <v>0</v>
       </c>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="15" t="s">
+      <c r="P28" s="9"/>
+      <c r="Q28" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="8" t="s">
+      <c r="R28" s="7" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2739,17 +2755,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF90C4-3DFD-4EFD-8B09-A2F83493DCEA}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2815,7 +2831,7 @@
         <v>HUC8</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T2" t="s">
         <v>0</v>
       </c>
@@ -2826,7 +2842,49 @@
         <v>Draft_MIP</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>193</v>
+      </c>
       <c r="T3" t="s">
         <v>1</v>
       </c>
@@ -2837,7 +2895,7 @@
         <v>FP_MIP</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T4" t="s">
         <v>2</v>
       </c>
@@ -2848,7 +2906,7 @@
         <v>FRP</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T5" t="s">
         <v>3</v>
       </c>
@@ -2859,7 +2917,7 @@
         <v>BFE_TODO</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T6" t="s">
         <v>4</v>
       </c>
@@ -2870,7 +2928,7 @@
         <v>P02a_Assign</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T7" t="s">
         <v>5</v>
       </c>
@@ -2881,7 +2939,7 @@
         <v>P01_MM</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T8" t="s">
         <v>6</v>
       </c>
@@ -2892,7 +2950,7 @@
         <v>Hydra_MIP</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T9" t="s">
         <v>7</v>
       </c>
@@ -2903,7 +2961,7 @@
         <v>which_grid</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T10" t="s">
         <v>8</v>
       </c>
@@ -2914,7 +2972,7 @@
         <v>Name</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T11" t="s">
         <v>9</v>
       </c>
@@ -2925,7 +2983,7 @@
         <v>Has AECOM Tie</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T12" t="s">
         <v>10</v>
       </c>
@@ -2936,7 +2994,7 @@
         <v>RAW_Grd_MM</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T13" t="s">
         <v>11</v>
       </c>
@@ -2947,7 +3005,7 @@
         <v>DFIRM_Grd_MM</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T14" t="s">
         <v>12</v>
       </c>
@@ -2958,7 +3016,7 @@
         <v>Addl_Grd_MM</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T15" t="s">
         <v>13</v>
       </c>
@@ -2969,7 +3027,7 @@
         <v>Prod Stage</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T16" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +3038,7 @@
         <v>P01 Analyst</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T17" t="s">
         <v>15</v>
       </c>
@@ -2991,7 +3049,7 @@
         <v>TO_Area</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T18" t="s">
         <v>16</v>
       </c>
@@ -3002,7 +3060,7 @@
         <v>Model Complete</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T19" t="s">
         <v>17</v>
       </c>
@@ -3013,7 +3071,7 @@
         <v>Notes</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T20" t="s">
         <v>18</v>
       </c>
@@ -3021,7 +3079,7 @@
         <v>MIP_Case</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T21" t="s">
         <v>19</v>
       </c>
@@ -3029,12 +3087,12 @@
         <v>FRP_Perc_Complete</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -3101,5 +3159,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>